<commit_message>
Calibration sheet start year electricity generation adjusted and land/BLAPE files updated
</commit_message>
<xml_diff>
--- a/InputData/land/BLAPE/BAU LULUCF Anthro Pollutant Emis.xlsx
+++ b/InputData/land/BLAPE/BAU LULUCF Anthro Pollutant Emis.xlsx
@@ -1,26 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shelley\Dropbox (Energy Innovation)\PC (2)\Documents\GitHub_Repositories\eps-california\InputData\land\BLAPE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ChrisB\Dropbox (Energy Innovation)\Desktop\Current CA EPS update\Land\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B96D6C32-A795-49FF-8295-C00E27E87088}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{59D1EA82-802F-445B-AEDD-4C5CE0A76087}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15345" yWindow="-16320" windowWidth="29040" windowHeight="15840" tabRatio="790" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="790" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="MN_GHG Data" sheetId="2" state="hidden" r:id="rId2"/>
-    <sheet name="Calcs" sheetId="12" r:id="rId3"/>
-    <sheet name="data from RPEpUACE" sheetId="6" r:id="rId4"/>
-    <sheet name="BLAPE" sheetId="7" r:id="rId5"/>
+    <sheet name="Empirical" sheetId="12" r:id="rId3"/>
+    <sheet name="Long run trend" sheetId="13" r:id="rId4"/>
+    <sheet name="Transition to long run trend" sheetId="14" r:id="rId5"/>
+    <sheet name="data from RPEpUACE" sheetId="6" r:id="rId6"/>
+    <sheet name="BLAPE" sheetId="7" r:id="rId7"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId6"/>
+    <externalReference r:id="rId8"/>
   </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'MN_GHG Data'!$A$1:$Q$1202</definedName>
@@ -41,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13786" uniqueCount="326">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13807" uniqueCount="342">
   <si>
     <t>BLAPE BAU LULUCF Anthropogenic Pollutant Emissions</t>
   </si>
@@ -859,9 +861,6 @@
     <t>F gases (g CO2e)</t>
   </si>
   <si>
-    <t>Wildfire adjustments for 2016-2020</t>
-  </si>
-  <si>
     <t>Average CO2 emissions from 2002 to 2015</t>
   </si>
   <si>
@@ -1020,19 +1019,77 @@
   <si>
     <t>year's wildfire emission estimates and the average historical wildfire emissions from 2001 to 2015.</t>
   </si>
+  <si>
+    <t>ecosystem carbon was projected to decline by a cumulative -479.2 Tg C by 2100 (-5.1 Tg C/year)."</t>
+  </si>
+  <si>
+    <t>2021 estimate based on wildfire acres burned</t>
+  </si>
+  <si>
+    <t>acres</t>
+  </si>
+  <si>
+    <t>CO2 emitted</t>
+  </si>
+  <si>
+    <t>Estimate based on ratio</t>
+  </si>
+  <si>
+    <t>2021 estimate</t>
+  </si>
+  <si>
+    <t>average 2010-2021</t>
+  </si>
+  <si>
+    <t>BLAPE</t>
+  </si>
+  <si>
+    <t>Assume 2022 equals average of last 10 years. In 2023, starts trending to long run average, reached in 2030.</t>
+  </si>
+  <si>
+    <t>Trend</t>
+  </si>
+  <si>
+    <t>Tg</t>
+  </si>
+  <si>
+    <t>Scatter plot</t>
+  </si>
+  <si>
+    <t>coeff</t>
+  </si>
+  <si>
+    <t>intercept</t>
+  </si>
+  <si>
+    <t>ln(x)</t>
+  </si>
+  <si>
+    <t>Imputed</t>
+  </si>
+  <si>
+    <t>Convert C to CO2</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1266,78 +1323,81 @@
   </borders>
   <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1"/>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="1" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="1" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="11" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1"/>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1"/>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="4"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="4" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="4" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="5" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="4"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="4" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="4" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="5" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="3" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="3" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="6"/>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="5" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="6"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="4" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="4" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="3" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="3" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="4" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="4" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="4" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="4" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="4" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="4" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="7" xfId="4" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="8" xfId="4" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="4" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="4" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="5" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="4" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="4" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="5" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="5" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="4" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="4" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="2" applyFont="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -1359,6 +1419,905 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="log"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Transition to long run trend'!$B$10:$C$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Transition to long run trend'!$B$11:$C$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>63.680905329200797</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>18.7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-04E4-4DB2-95B0-099920586828}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="722018336"/>
+        <c:axId val="722020632"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="722018336"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="722020632"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="722020632"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="722018336"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1402,6 +2361,91 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>162084</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>309751</xdr:colOff>
+      <xdr:row>82</xdr:row>
+      <xdr:rowOff>118531</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AB8BEE36-1E46-4104-ACA9-6036FA39474A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="12823984"/>
+          <a:ext cx="4761101" cy="2090047"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>501650</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>130175</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>450850</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A53C1F18-E3E9-4F79-902E-8CA448F54EA9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1685,7 +2729,7 @@
     </row>
     <row r="3" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B3" s="2" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
@@ -1695,23 +2739,23 @@
     </row>
     <row r="5" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B5" s="2" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B6" s="38" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B7" s="2" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="14" x14ac:dyDescent="0.3"/>
     <row r="9" spans="1:3" s="15" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B9" s="2" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="10" spans="1:3" s="15" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
@@ -1721,17 +2765,17 @@
     </row>
     <row r="11" spans="1:3" s="15" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B11" s="2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="12" spans="1:3" s="15" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B12" s="39" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="13" spans="1:3" s="15" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B13" s="2" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="14" spans="1:3" s="15" customFormat="1" ht="14" x14ac:dyDescent="0.3"/>
@@ -1749,12 +2793,12 @@
     <row r="18" spans="1:9" ht="14" x14ac:dyDescent="0.3"/>
     <row r="19" spans="1:9" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A20" s="35" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B20" s="35"/>
       <c r="C20" s="35"/>
@@ -1767,7 +2811,7 @@
     </row>
     <row r="21" spans="1:9" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A21" s="35" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B21" s="35"/>
       <c r="C21" s="35"/>
@@ -1780,7 +2824,7 @@
     </row>
     <row r="22" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="37" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B22" s="35"/>
       <c r="C22" s="35"/>
@@ -1793,7 +2837,7 @@
     </row>
     <row r="23" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="37" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B23" s="35"/>
       <c r="C23" s="35"/>
@@ -60686,22 +61730,24 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{329D65DF-0E8F-410C-BB90-5CF6AFECDB3B}">
-  <dimension ref="B2:CZ67"/>
+  <dimension ref="A2:CZ70"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q35" sqref="Q35"/>
+    <sheetView topLeftCell="A51" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="M48" sqref="M48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="11" width="8.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.08203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="11" width="8.75" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10" customWidth="1"/>
     <col min="13" max="16" width="8.75" bestFit="1" customWidth="1"/>
     <col min="17" max="19" width="10.83203125" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="11.4140625" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="10.83203125" bestFit="1" customWidth="1"/>
-    <col min="22" max="101" width="8.75" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="13.58203125" customWidth="1"/>
+    <col min="23" max="101" width="8.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:15" ht="14.5" x14ac:dyDescent="0.35">
@@ -60719,7 +61765,7 @@
     </row>
     <row r="3" spans="2:15" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B3" s="22" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C3" s="16"/>
       <c r="D3" s="16"/>
@@ -60731,7 +61777,7 @@
       <c r="J3" s="16"/>
       <c r="K3" s="16"/>
       <c r="L3" s="29" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="M3" s="16">
         <f>10^12</f>
@@ -60739,12 +61785,12 @@
       </c>
       <c r="N3" s="16"/>
       <c r="O3" s="16" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="4" spans="2:15" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B4" s="16" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C4" s="16"/>
       <c r="D4" s="16"/>
@@ -60762,62 +61808,62 @@
     <row r="5" spans="2:15" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B5" s="16"/>
       <c r="C5" s="16" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D5" s="16"/>
       <c r="E5" s="16"/>
       <c r="F5" s="16"/>
       <c r="G5" s="16" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="H5" s="16"/>
       <c r="I5" s="16"/>
       <c r="J5" s="16" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="K5" s="16"/>
       <c r="L5" s="16"/>
       <c r="N5" s="16" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="O5" s="16"/>
     </row>
     <row r="6" spans="2:15" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B6" s="16" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D6" s="16" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E6" s="16" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="F6" s="16" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="G6" s="16" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="H6" s="16" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="I6" s="16" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="J6" s="16" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="K6" s="26" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="L6" s="16" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="N6" s="16" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="O6" s="16"/>
     </row>
@@ -60838,25 +61884,25 @@
         <v>4823.1000000000004</v>
       </c>
       <c r="G7" s="16" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="H7" s="16" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="I7" s="16" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="J7" s="16" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="K7" s="27" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="L7" s="16" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="N7" s="16" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="O7" s="16"/>
     </row>
@@ -60895,7 +61941,7 @@
         <v>1.8</v>
       </c>
       <c r="N8" s="16" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="O8" s="16"/>
     </row>
@@ -60934,7 +61980,7 @@
         <v>2.9</v>
       </c>
       <c r="N9" s="16" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="O9" s="16"/>
     </row>
@@ -60973,7 +62019,7 @@
         <v>3.9</v>
       </c>
       <c r="N10" s="16" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="O10" s="16"/>
     </row>
@@ -61012,7 +62058,7 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="N11" s="16" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="O11" s="16"/>
     </row>
@@ -61086,7 +62132,7 @@
         <v>7.1</v>
       </c>
       <c r="N13" s="34" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="14" spans="2:15" ht="14.5" x14ac:dyDescent="0.35">
@@ -61124,7 +62170,7 @@
         <v>8.1</v>
       </c>
       <c r="N14" s="34" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="15" spans="2:15" ht="14.5" x14ac:dyDescent="0.35">
@@ -61162,7 +62208,7 @@
         <v>8.6999999999999993</v>
       </c>
       <c r="N15" s="34" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="16" spans="2:15" ht="14.5" x14ac:dyDescent="0.35">
@@ -61200,7 +62246,7 @@
         <v>9.4</v>
       </c>
       <c r="N16" s="34" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="17" spans="2:104" ht="14.5" x14ac:dyDescent="0.35">
@@ -61274,7 +62320,7 @@
         <v>10.199999999999999</v>
       </c>
       <c r="N18" s="34" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="19" spans="2:104" ht="14.5" x14ac:dyDescent="0.35">
@@ -61312,7 +62358,7 @@
         <v>11.2</v>
       </c>
       <c r="N19" s="34" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="20" spans="2:104" ht="14.5" x14ac:dyDescent="0.35">
@@ -61350,7 +62396,7 @@
         <v>12.2</v>
       </c>
       <c r="N20" s="34" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="21" spans="2:104" ht="14.5" x14ac:dyDescent="0.35">
@@ -61404,23 +62450,23 @@
       <c r="K22" s="16"/>
       <c r="L22" s="16"/>
       <c r="N22" s="34" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="23" spans="2:104" ht="14.5" x14ac:dyDescent="0.35">
       <c r="N23" s="34" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="25" spans="2:104" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B25" s="16"/>
       <c r="C25" s="29" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="26" spans="2:104" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B26" s="16" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C26" s="25">
         <v>2002</v>
@@ -61722,7 +62768,7 @@
     </row>
     <row r="27" spans="2:104" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B27" s="29" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C27" s="29">
         <f>-1*K8</f>
@@ -61780,344 +62826,344 @@
         <f>-1*K21</f>
         <v>44.6</v>
       </c>
-      <c r="Q27" s="36">
-        <f>5.6+(C67/$M$3)</f>
-        <v>2.6142857142857143</v>
-      </c>
-      <c r="R27" s="36">
-        <f>5.6+(D67/$M$3)</f>
-        <v>23.414285714285711</v>
-      </c>
-      <c r="S27" s="36">
-        <f>5.6+(E67/$M$3)</f>
-        <v>31.214285714285715</v>
-      </c>
-      <c r="T27" s="36">
-        <f>5.6+(F67/$M$3)</f>
-        <v>-3.0857142857142854</v>
-      </c>
-      <c r="U27" s="36">
-        <f>5.6+(G67/$M$3)</f>
-        <v>98.814285714285717</v>
+      <c r="Q27" s="36" t="e">
+        <f>5.6+(#REF!/$M$3)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="R27" s="36" t="e">
+        <f>5.6+(#REF!/$M$3)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="S27" s="36" t="e">
+        <f>5.6+(#REF!/$M$3)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="T27" s="36" t="e">
+        <f>5.6+(#REF!/$M$3)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="U27" s="36" t="e">
+        <f>5.6+(#REF!/$M$3)</f>
+        <v>#REF!</v>
       </c>
       <c r="V27" s="35">
-        <f>5.6</f>
+        <f t="shared" ref="V27:BA27" si="0">5.6</f>
         <v>5.6</v>
       </c>
       <c r="W27" s="35">
-        <f>5.6</f>
+        <f t="shared" si="0"/>
         <v>5.6</v>
       </c>
       <c r="X27" s="35">
-        <f>5.6</f>
+        <f t="shared" si="0"/>
         <v>5.6</v>
       </c>
       <c r="Y27" s="35">
-        <f>5.6</f>
+        <f t="shared" si="0"/>
         <v>5.6</v>
       </c>
       <c r="Z27" s="35">
-        <f>5.6</f>
+        <f t="shared" si="0"/>
         <v>5.6</v>
       </c>
       <c r="AA27" s="35">
-        <f>5.6</f>
+        <f t="shared" si="0"/>
         <v>5.6</v>
       </c>
       <c r="AB27" s="35">
-        <f>5.6</f>
+        <f t="shared" si="0"/>
         <v>5.6</v>
       </c>
       <c r="AC27" s="35">
-        <f>5.6</f>
+        <f t="shared" si="0"/>
         <v>5.6</v>
       </c>
       <c r="AD27" s="35">
-        <f>5.6</f>
+        <f t="shared" si="0"/>
         <v>5.6</v>
       </c>
       <c r="AE27" s="35">
-        <f>5.6</f>
+        <f t="shared" si="0"/>
         <v>5.6</v>
       </c>
       <c r="AF27" s="35">
-        <f>5.6</f>
+        <f t="shared" si="0"/>
         <v>5.6</v>
       </c>
       <c r="AG27" s="35">
-        <f>5.6</f>
+        <f t="shared" si="0"/>
         <v>5.6</v>
       </c>
       <c r="AH27" s="35">
-        <f>5.6</f>
+        <f t="shared" si="0"/>
         <v>5.6</v>
       </c>
       <c r="AI27" s="35">
-        <f>5.6</f>
+        <f t="shared" si="0"/>
         <v>5.6</v>
       </c>
       <c r="AJ27" s="35">
-        <f>5.6</f>
+        <f t="shared" si="0"/>
         <v>5.6</v>
       </c>
       <c r="AK27" s="35">
-        <f>5.6</f>
+        <f t="shared" si="0"/>
         <v>5.6</v>
       </c>
       <c r="AL27" s="35">
-        <f>5.6</f>
+        <f t="shared" si="0"/>
         <v>5.6</v>
       </c>
       <c r="AM27" s="35">
-        <f>5.6</f>
+        <f t="shared" si="0"/>
         <v>5.6</v>
       </c>
       <c r="AN27" s="35">
-        <f>5.6</f>
+        <f t="shared" si="0"/>
         <v>5.6</v>
       </c>
       <c r="AO27" s="35">
-        <f>5.6</f>
+        <f t="shared" si="0"/>
         <v>5.6</v>
       </c>
       <c r="AP27" s="35">
-        <f>5.6</f>
+        <f t="shared" si="0"/>
         <v>5.6</v>
       </c>
       <c r="AQ27" s="35">
-        <f>5.6</f>
+        <f t="shared" si="0"/>
         <v>5.6</v>
       </c>
       <c r="AR27" s="35">
-        <f>5.6</f>
+        <f t="shared" si="0"/>
         <v>5.6</v>
       </c>
       <c r="AS27" s="35">
-        <f>5.6</f>
+        <f t="shared" si="0"/>
         <v>5.6</v>
       </c>
       <c r="AT27" s="35">
-        <f>5.6</f>
+        <f t="shared" si="0"/>
         <v>5.6</v>
       </c>
       <c r="AU27" s="35">
-        <f>5.6</f>
+        <f t="shared" si="0"/>
         <v>5.6</v>
       </c>
       <c r="AV27" s="35">
-        <f>5.6</f>
+        <f t="shared" si="0"/>
         <v>5.6</v>
       </c>
       <c r="AW27" s="35">
-        <f>5.6</f>
+        <f t="shared" si="0"/>
         <v>5.6</v>
       </c>
       <c r="AX27" s="35">
-        <f>5.6</f>
+        <f t="shared" si="0"/>
         <v>5.6</v>
       </c>
       <c r="AY27" s="35">
-        <f>5.6</f>
+        <f t="shared" si="0"/>
         <v>5.6</v>
       </c>
       <c r="AZ27" s="35">
-        <f>5.6</f>
+        <f t="shared" si="0"/>
         <v>5.6</v>
       </c>
       <c r="BA27" s="35">
-        <f>5.6</f>
+        <f t="shared" si="0"/>
         <v>5.6</v>
       </c>
       <c r="BB27" s="35">
-        <f>5.6</f>
+        <f t="shared" ref="BB27:CG27" si="1">5.6</f>
         <v>5.6</v>
       </c>
       <c r="BC27" s="35">
-        <f>5.6</f>
+        <f t="shared" si="1"/>
         <v>5.6</v>
       </c>
       <c r="BD27" s="35">
-        <f>5.6</f>
+        <f t="shared" si="1"/>
         <v>5.6</v>
       </c>
       <c r="BE27" s="35">
-        <f>5.6</f>
+        <f t="shared" si="1"/>
         <v>5.6</v>
       </c>
       <c r="BF27" s="35">
-        <f>5.6</f>
+        <f t="shared" si="1"/>
         <v>5.6</v>
       </c>
       <c r="BG27" s="35">
-        <f>5.6</f>
+        <f t="shared" si="1"/>
         <v>5.6</v>
       </c>
       <c r="BH27" s="35">
-        <f>5.6</f>
+        <f t="shared" si="1"/>
         <v>5.6</v>
       </c>
       <c r="BI27" s="35">
-        <f>5.6</f>
+        <f t="shared" si="1"/>
         <v>5.6</v>
       </c>
       <c r="BJ27" s="35">
-        <f>5.6</f>
+        <f t="shared" si="1"/>
         <v>5.6</v>
       </c>
       <c r="BK27" s="35">
-        <f>5.6</f>
+        <f t="shared" si="1"/>
         <v>5.6</v>
       </c>
       <c r="BL27" s="35">
-        <f>5.6</f>
+        <f t="shared" si="1"/>
         <v>5.6</v>
       </c>
       <c r="BM27" s="35">
-        <f>5.6</f>
+        <f t="shared" si="1"/>
         <v>5.6</v>
       </c>
       <c r="BN27" s="35">
-        <f>5.6</f>
+        <f t="shared" si="1"/>
         <v>5.6</v>
       </c>
       <c r="BO27" s="35">
-        <f>5.6</f>
+        <f t="shared" si="1"/>
         <v>5.6</v>
       </c>
       <c r="BP27" s="35">
-        <f>5.6</f>
+        <f t="shared" si="1"/>
         <v>5.6</v>
       </c>
       <c r="BQ27" s="35">
-        <f>5.6</f>
+        <f t="shared" si="1"/>
         <v>5.6</v>
       </c>
       <c r="BR27" s="35">
-        <f>5.6</f>
+        <f t="shared" si="1"/>
         <v>5.6</v>
       </c>
       <c r="BS27" s="35">
-        <f>5.6</f>
+        <f t="shared" si="1"/>
         <v>5.6</v>
       </c>
       <c r="BT27" s="35">
-        <f>5.6</f>
+        <f t="shared" si="1"/>
         <v>5.6</v>
       </c>
       <c r="BU27" s="35">
-        <f>5.6</f>
+        <f t="shared" si="1"/>
         <v>5.6</v>
       </c>
       <c r="BV27" s="35">
-        <f>5.6</f>
+        <f t="shared" si="1"/>
         <v>5.6</v>
       </c>
       <c r="BW27" s="35">
-        <f>5.6</f>
+        <f t="shared" si="1"/>
         <v>5.6</v>
       </c>
       <c r="BX27" s="35">
-        <f>5.6</f>
+        <f t="shared" si="1"/>
         <v>5.6</v>
       </c>
       <c r="BY27" s="35">
-        <f>5.6</f>
+        <f t="shared" si="1"/>
         <v>5.6</v>
       </c>
       <c r="BZ27" s="35">
-        <f>5.6</f>
+        <f t="shared" si="1"/>
         <v>5.6</v>
       </c>
       <c r="CA27" s="35">
-        <f>5.6</f>
+        <f t="shared" si="1"/>
         <v>5.6</v>
       </c>
       <c r="CB27" s="35">
-        <f>5.6</f>
+        <f t="shared" si="1"/>
         <v>5.6</v>
       </c>
       <c r="CC27" s="35">
-        <f>5.6</f>
+        <f t="shared" si="1"/>
         <v>5.6</v>
       </c>
       <c r="CD27" s="35">
-        <f>5.6</f>
+        <f t="shared" si="1"/>
         <v>5.6</v>
       </c>
       <c r="CE27" s="35">
-        <f>5.6</f>
+        <f t="shared" si="1"/>
         <v>5.6</v>
       </c>
       <c r="CF27" s="35">
-        <f>5.6</f>
+        <f t="shared" si="1"/>
         <v>5.6</v>
       </c>
       <c r="CG27" s="35">
-        <f>5.6</f>
+        <f t="shared" si="1"/>
         <v>5.6</v>
       </c>
       <c r="CH27" s="35">
-        <f>5.6</f>
+        <f t="shared" ref="CH27:CW27" si="2">5.6</f>
         <v>5.6</v>
       </c>
       <c r="CI27" s="35">
-        <f>5.6</f>
+        <f t="shared" si="2"/>
         <v>5.6</v>
       </c>
       <c r="CJ27" s="35">
-        <f>5.6</f>
+        <f t="shared" si="2"/>
         <v>5.6</v>
       </c>
       <c r="CK27" s="35">
-        <f>5.6</f>
+        <f t="shared" si="2"/>
         <v>5.6</v>
       </c>
       <c r="CL27" s="35">
-        <f>5.6</f>
+        <f t="shared" si="2"/>
         <v>5.6</v>
       </c>
       <c r="CM27" s="35">
-        <f>5.6</f>
+        <f t="shared" si="2"/>
         <v>5.6</v>
       </c>
       <c r="CN27" s="35">
-        <f>5.6</f>
+        <f t="shared" si="2"/>
         <v>5.6</v>
       </c>
       <c r="CO27" s="35">
-        <f>5.6</f>
+        <f t="shared" si="2"/>
         <v>5.6</v>
       </c>
       <c r="CP27" s="35">
-        <f>5.6</f>
+        <f t="shared" si="2"/>
         <v>5.6</v>
       </c>
       <c r="CQ27" s="35">
-        <f>5.6</f>
+        <f t="shared" si="2"/>
         <v>5.6</v>
       </c>
       <c r="CR27" s="35">
-        <f>5.6</f>
+        <f t="shared" si="2"/>
         <v>5.6</v>
       </c>
       <c r="CS27" s="35">
-        <f>5.6</f>
+        <f t="shared" si="2"/>
         <v>5.6</v>
       </c>
       <c r="CT27" s="35">
-        <f>5.6</f>
+        <f t="shared" si="2"/>
         <v>5.6</v>
       </c>
       <c r="CU27" s="35">
-        <f>5.6</f>
+        <f t="shared" si="2"/>
         <v>5.6</v>
       </c>
       <c r="CV27" s="35">
-        <f>5.6</f>
+        <f t="shared" si="2"/>
         <v>5.6</v>
       </c>
       <c r="CW27" s="35">
-        <f>5.6</f>
+        <f t="shared" si="2"/>
         <v>5.6</v>
       </c>
       <c r="CX27" s="10"/>
@@ -62133,395 +63179,395 @@
         <v>27300000000000</v>
       </c>
       <c r="D28" s="29">
-        <f t="shared" ref="D28:BO28" si="0">D27*$M$3</f>
+        <f t="shared" ref="D28:BO28" si="3">D27*$M$3</f>
         <v>6300000000000</v>
       </c>
       <c r="E28" s="29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>-7200000000000</v>
       </c>
       <c r="F28" s="29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>-38600000000000</v>
       </c>
       <c r="G28" s="29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>-4500000000000</v>
       </c>
       <c r="H28" s="29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>50100000000000</v>
       </c>
       <c r="I28" s="29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>28700000000000</v>
       </c>
       <c r="J28" s="29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>19200000000000</v>
       </c>
       <c r="K28" s="29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>-60100000000000</v>
       </c>
       <c r="L28" s="29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>4099999999999.9995</v>
       </c>
       <c r="M28" s="29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>6200000000000</v>
       </c>
       <c r="N28" s="29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>89800000000000</v>
       </c>
       <c r="O28" s="29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>22500000000000</v>
       </c>
       <c r="P28" s="29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>44600000000000</v>
       </c>
-      <c r="Q28" s="29">
-        <f t="shared" si="0"/>
-        <v>2614285714285.7144</v>
-      </c>
-      <c r="R28" s="29">
-        <f t="shared" si="0"/>
-        <v>23414285714285.711</v>
-      </c>
-      <c r="S28" s="29">
-        <f t="shared" si="0"/>
-        <v>31214285714285.715</v>
-      </c>
-      <c r="T28" s="29">
-        <f t="shared" si="0"/>
-        <v>-3085714285714.2856</v>
-      </c>
-      <c r="U28" s="29">
-        <f t="shared" si="0"/>
-        <v>98814285714285.719</v>
+      <c r="Q28" s="29" t="e">
+        <f t="shared" si="3"/>
+        <v>#REF!</v>
+      </c>
+      <c r="R28" s="29" t="e">
+        <f t="shared" si="3"/>
+        <v>#REF!</v>
+      </c>
+      <c r="S28" s="29" t="e">
+        <f t="shared" si="3"/>
+        <v>#REF!</v>
+      </c>
+      <c r="T28" s="29" t="e">
+        <f t="shared" si="3"/>
+        <v>#REF!</v>
+      </c>
+      <c r="U28" s="29" t="e">
+        <f t="shared" si="3"/>
+        <v>#REF!</v>
       </c>
       <c r="V28" s="29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>5600000000000</v>
       </c>
       <c r="W28" s="29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>5600000000000</v>
       </c>
       <c r="X28" s="29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>5600000000000</v>
       </c>
       <c r="Y28" s="29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>5600000000000</v>
       </c>
       <c r="Z28" s="29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>5600000000000</v>
       </c>
       <c r="AA28" s="29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>5600000000000</v>
       </c>
       <c r="AB28" s="29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>5600000000000</v>
       </c>
       <c r="AC28" s="29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>5600000000000</v>
       </c>
       <c r="AD28" s="29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>5600000000000</v>
       </c>
       <c r="AE28" s="29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>5600000000000</v>
       </c>
       <c r="AF28" s="29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>5600000000000</v>
       </c>
       <c r="AG28" s="29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>5600000000000</v>
       </c>
       <c r="AH28" s="29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>5600000000000</v>
       </c>
       <c r="AI28" s="29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>5600000000000</v>
       </c>
       <c r="AJ28" s="29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>5600000000000</v>
       </c>
       <c r="AK28" s="29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>5600000000000</v>
       </c>
       <c r="AL28" s="29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>5600000000000</v>
       </c>
       <c r="AM28" s="29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>5600000000000</v>
       </c>
       <c r="AN28" s="29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>5600000000000</v>
       </c>
       <c r="AO28" s="29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>5600000000000</v>
       </c>
       <c r="AP28" s="29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>5600000000000</v>
       </c>
       <c r="AQ28" s="29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>5600000000000</v>
       </c>
       <c r="AR28" s="29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>5600000000000</v>
       </c>
       <c r="AS28" s="29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>5600000000000</v>
       </c>
       <c r="AT28" s="29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>5600000000000</v>
       </c>
       <c r="AU28" s="29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>5600000000000</v>
       </c>
       <c r="AV28" s="29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>5600000000000</v>
       </c>
       <c r="AW28" s="29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>5600000000000</v>
       </c>
       <c r="AX28" s="29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>5600000000000</v>
       </c>
       <c r="AY28" s="29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>5600000000000</v>
       </c>
       <c r="AZ28" s="29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>5600000000000</v>
       </c>
       <c r="BA28" s="29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>5600000000000</v>
       </c>
       <c r="BB28" s="29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>5600000000000</v>
       </c>
       <c r="BC28" s="29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>5600000000000</v>
       </c>
       <c r="BD28" s="29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>5600000000000</v>
       </c>
       <c r="BE28" s="29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>5600000000000</v>
       </c>
       <c r="BF28" s="29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>5600000000000</v>
       </c>
       <c r="BG28" s="29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>5600000000000</v>
       </c>
       <c r="BH28" s="29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>5600000000000</v>
       </c>
       <c r="BI28" s="29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>5600000000000</v>
       </c>
       <c r="BJ28" s="29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>5600000000000</v>
       </c>
       <c r="BK28" s="29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>5600000000000</v>
       </c>
       <c r="BL28" s="29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>5600000000000</v>
       </c>
       <c r="BM28" s="29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>5600000000000</v>
       </c>
       <c r="BN28" s="29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>5600000000000</v>
       </c>
       <c r="BO28" s="29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>5600000000000</v>
       </c>
       <c r="BP28" s="29">
-        <f t="shared" ref="BP28:CW28" si="1">BP27*$M$3</f>
+        <f t="shared" ref="BP28:CW28" si="4">BP27*$M$3</f>
         <v>5600000000000</v>
       </c>
       <c r="BQ28" s="29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>5600000000000</v>
       </c>
       <c r="BR28" s="29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>5600000000000</v>
       </c>
       <c r="BS28" s="29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>5600000000000</v>
       </c>
       <c r="BT28" s="29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>5600000000000</v>
       </c>
       <c r="BU28" s="29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>5600000000000</v>
       </c>
       <c r="BV28" s="29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>5600000000000</v>
       </c>
       <c r="BW28" s="29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>5600000000000</v>
       </c>
       <c r="BX28" s="29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>5600000000000</v>
       </c>
       <c r="BY28" s="29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>5600000000000</v>
       </c>
       <c r="BZ28" s="29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>5600000000000</v>
       </c>
       <c r="CA28" s="29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>5600000000000</v>
       </c>
       <c r="CB28" s="29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>5600000000000</v>
       </c>
       <c r="CC28" s="29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>5600000000000</v>
       </c>
       <c r="CD28" s="29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>5600000000000</v>
       </c>
       <c r="CE28" s="29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>5600000000000</v>
       </c>
       <c r="CF28" s="29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>5600000000000</v>
       </c>
       <c r="CG28" s="29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>5600000000000</v>
       </c>
       <c r="CH28" s="29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>5600000000000</v>
       </c>
       <c r="CI28" s="29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>5600000000000</v>
       </c>
       <c r="CJ28" s="29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>5600000000000</v>
       </c>
       <c r="CK28" s="29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>5600000000000</v>
       </c>
       <c r="CL28" s="29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>5600000000000</v>
       </c>
       <c r="CM28" s="29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>5600000000000</v>
       </c>
       <c r="CN28" s="29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>5600000000000</v>
       </c>
       <c r="CO28" s="29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>5600000000000</v>
       </c>
       <c r="CP28" s="29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>5600000000000</v>
       </c>
       <c r="CQ28" s="29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>5600000000000</v>
       </c>
       <c r="CR28" s="29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>5600000000000</v>
       </c>
       <c r="CS28" s="29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>5600000000000</v>
       </c>
       <c r="CT28" s="29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>5600000000000</v>
       </c>
       <c r="CU28" s="29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>5600000000000</v>
       </c>
       <c r="CV28" s="29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>5600000000000</v>
       </c>
       <c r="CW28" s="29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>5600000000000</v>
       </c>
     </row>
@@ -62530,18 +63576,18 @@
     </row>
     <row r="31" spans="2:104" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B31" s="22" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="32" spans="2:104" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B32" s="16" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="59" spans="2:21" ht="14.5" x14ac:dyDescent="0.35">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="59" spans="2:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B59" s="16"/>
       <c r="C59" s="16" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D59" s="16"/>
       <c r="E59" s="16"/>
@@ -62562,9 +63608,9 @@
       <c r="T59" s="16"/>
       <c r="U59" s="16"/>
     </row>
-    <row r="60" spans="2:21" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="60" spans="2:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B60" s="16" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C60" s="21">
         <v>2002</v>
@@ -62623,10 +63669,13 @@
       <c r="U60" s="19">
         <v>2020</v>
       </c>
-    </row>
-    <row r="61" spans="2:21" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="V60" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="61" spans="2:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B61" s="16" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C61" s="16">
         <f>13.5</f>
@@ -62705,7 +63754,7 @@
         <v>106.7</v>
       </c>
     </row>
-    <row r="62" spans="2:21" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="62" spans="2:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B62" s="16" t="s">
         <v>249</v>
       </c>
@@ -62714,81 +63763,85 @@
         <v>13500000000000</v>
       </c>
       <c r="D62" s="16">
-        <f t="shared" ref="D62:U62" si="2">D61*$M$3</f>
+        <f t="shared" ref="D62:U62" si="5">D61*$M$3</f>
         <v>18300000000000</v>
       </c>
       <c r="E62" s="16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>5200000000000</v>
       </c>
       <c r="F62" s="16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>2000000000000</v>
       </c>
       <c r="G62" s="16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>12600000000000</v>
       </c>
       <c r="H62" s="16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>19900000000000</v>
       </c>
       <c r="I62" s="16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>41700000000000</v>
       </c>
       <c r="J62" s="16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>8800000000000</v>
       </c>
       <c r="K62" s="16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1300000000000</v>
       </c>
       <c r="L62" s="16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>3100000000000</v>
       </c>
       <c r="M62" s="16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>11300000000000</v>
       </c>
       <c r="N62" s="16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>14700000000000</v>
       </c>
       <c r="O62" s="16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>17200000000000</v>
       </c>
       <c r="P62" s="16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>19200000000000</v>
       </c>
       <c r="Q62" s="16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>10500000000000</v>
       </c>
       <c r="R62" s="16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>31300000000000</v>
       </c>
       <c r="S62" s="16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>39100000000000</v>
       </c>
       <c r="T62" s="16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>4800000000000</v>
       </c>
       <c r="U62" s="16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>106700000000000</v>
       </c>
-    </row>
-    <row r="63" spans="2:21" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="V62">
+        <f>$D$69</f>
+        <v>63680905329200.797</v>
+      </c>
+    </row>
+    <row r="63" spans="2:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B63" s="17" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C63" s="17"/>
       <c r="D63" s="18"/>
@@ -62813,56 +63866,54 @@
       <c r="T63" s="16"/>
       <c r="U63" s="16"/>
     </row>
-    <row r="65" spans="3:8" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="C65" s="16" t="s">
-        <v>272</v>
-      </c>
-      <c r="D65" s="16"/>
-      <c r="E65" s="16"/>
-      <c r="F65" s="16"/>
-      <c r="G65" s="16"/>
-      <c r="H65" s="16"/>
-    </row>
-    <row r="66" spans="3:8" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="C66" s="30">
-        <v>2016</v>
-      </c>
-      <c r="D66" s="30">
-        <v>2017</v>
-      </c>
-      <c r="E66" s="30">
-        <v>2018</v>
-      </c>
-      <c r="F66" s="30">
-        <v>2019</v>
-      </c>
-      <c r="G66" s="31">
+    <row r="64" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="V64">
+        <f>AVERAGE(M62:V62)</f>
+        <v>31848090532920.082</v>
+      </c>
+      <c r="W64" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B68" t="s">
+        <v>327</v>
+      </c>
+      <c r="C68" t="s">
+        <v>328</v>
+      </c>
+      <c r="D68" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A69">
+        <v>2021</v>
+      </c>
+      <c r="B69">
+        <v>2568948</v>
+      </c>
+      <c r="D69">
+        <f>(B69/B70)*C70</f>
+        <v>63680905329200.797</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A70">
         <v>2020</v>
       </c>
-      <c r="H66" s="16"/>
-    </row>
-    <row r="67" spans="3:8" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="C67" s="16">
-        <f>Q62-$F$63</f>
-        <v>-2985714285714.2852</v>
-      </c>
-      <c r="D67" s="16">
-        <f t="shared" ref="D67:G67" si="3">R62-$F$63</f>
-        <v>17814285714285.715</v>
-      </c>
-      <c r="E67" s="16">
-        <f t="shared" si="3"/>
-        <v>25614285714285.715</v>
-      </c>
-      <c r="F67" s="16">
-        <f t="shared" si="3"/>
-        <v>-8685714285714.2852</v>
-      </c>
-      <c r="G67" s="16">
-        <f t="shared" si="3"/>
-        <v>93214285714285.719</v>
-      </c>
-      <c r="H67" s="16"/>
+      <c r="B70">
+        <v>4304379</v>
+      </c>
+      <c r="C70">
+        <f>U62</f>
+        <v>106700000000000</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -62875,11 +63926,463 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43B23769-14F1-4895-8312-1A8F72BFACC8}">
+  <dimension ref="A1:N12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="8.6640625" style="10"/>
+    <col min="2" max="2" width="11.75" style="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="10" width="8.75" style="10" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10" style="10" customWidth="1"/>
+    <col min="12" max="15" width="8.75" style="10" bestFit="1" customWidth="1"/>
+    <col min="16" max="18" width="10.83203125" style="10" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.4140625" style="10" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.83203125" style="10" bestFit="1" customWidth="1"/>
+    <col min="21" max="100" width="8.75" style="10" bestFit="1" customWidth="1"/>
+    <col min="101" max="16384" width="8.6640625" style="10"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A1" s="10" t="s">
+        <v>334</v>
+      </c>
+      <c r="B1" s="10">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>335</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="B2" s="13">
+        <f>B1*1000000000000</f>
+        <v>5100000000000</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>249</v>
+      </c>
+      <c r="I2" s="16"/>
+      <c r="J2" s="16"/>
+      <c r="K2" s="16"/>
+    </row>
+    <row r="3" spans="1:14" s="15" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="B3" s="41">
+        <f>B2*44/12</f>
+        <v>18700000000000</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>341</v>
+      </c>
+      <c r="I3" s="16"/>
+      <c r="J3" s="16"/>
+      <c r="K3" s="16"/>
+    </row>
+    <row r="4" spans="1:14" s="15" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="B4" s="41"/>
+      <c r="I4" s="16"/>
+      <c r="J4" s="16"/>
+      <c r="K4" s="16"/>
+    </row>
+    <row r="5" spans="1:14" s="15" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="B5" s="41"/>
+      <c r="I5" s="16"/>
+      <c r="J5" s="16"/>
+      <c r="K5" s="16"/>
+    </row>
+    <row r="6" spans="1:14" s="15" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="B6" s="41"/>
+      <c r="I6" s="16"/>
+      <c r="J6" s="16"/>
+      <c r="K6" s="16"/>
+    </row>
+    <row r="7" spans="1:14" s="15" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="34" t="s">
+        <v>316</v>
+      </c>
+      <c r="I7" s="16"/>
+      <c r="J7" s="16"/>
+      <c r="K7" s="16"/>
+    </row>
+    <row r="8" spans="1:14" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A8" s="40" t="s">
+        <v>325</v>
+      </c>
+      <c r="B8" s="16"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="16"/>
+      <c r="I8" s="16"/>
+      <c r="J8" s="16"/>
+      <c r="K8" s="29"/>
+      <c r="L8" s="16"/>
+      <c r="M8" s="16"/>
+      <c r="N8" s="16"/>
+    </row>
+    <row r="9" spans="1:14" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A9" s="34"/>
+      <c r="B9" s="16"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="16"/>
+      <c r="I9" s="16"/>
+      <c r="J9" s="16"/>
+      <c r="K9" s="16"/>
+      <c r="M9" s="16"/>
+      <c r="N9" s="16"/>
+    </row>
+    <row r="10" spans="1:14" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A10" s="22" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A11" s="16" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A12" s="16"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0EECC17-E131-4487-A30C-1F02F798DCF0}">
+  <dimension ref="A1:K15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3:K3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="3" width="12.08203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="15">
+        <v>2021</v>
+      </c>
+      <c r="C2" s="10">
+        <v>2022</v>
+      </c>
+      <c r="D2" s="10">
+        <f>C2+1</f>
+        <v>2023</v>
+      </c>
+      <c r="E2" s="10">
+        <f t="shared" ref="D2:K5" si="0">D2+1</f>
+        <v>2024</v>
+      </c>
+      <c r="F2" s="10">
+        <f t="shared" si="0"/>
+        <v>2025</v>
+      </c>
+      <c r="G2" s="10">
+        <f t="shared" si="0"/>
+        <v>2026</v>
+      </c>
+      <c r="H2" s="10">
+        <f t="shared" si="0"/>
+        <v>2027</v>
+      </c>
+      <c r="I2" s="10">
+        <f t="shared" si="0"/>
+        <v>2028</v>
+      </c>
+      <c r="J2" s="10">
+        <f t="shared" si="0"/>
+        <v>2029</v>
+      </c>
+      <c r="K2" s="10">
+        <f t="shared" si="0"/>
+        <v>2030</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="15" t="s">
+        <v>340</v>
+      </c>
+      <c r="B3" s="15">
+        <f>Empirical!D69</f>
+        <v>63680905329200.797</v>
+      </c>
+      <c r="C3" s="15">
+        <f>C6*1000000000000</f>
+        <v>50143835563664.266</v>
+      </c>
+      <c r="D3" s="15">
+        <f t="shared" ref="D3:K3" si="1">D6*1000000000000</f>
+        <v>42225102002311.813</v>
+      </c>
+      <c r="E3" s="15">
+        <f t="shared" si="1"/>
+        <v>36606671127328.531</v>
+      </c>
+      <c r="F3" s="15">
+        <f t="shared" si="1"/>
+        <v>32248677570162.016</v>
+      </c>
+      <c r="G3" s="15">
+        <f t="shared" si="1"/>
+        <v>28687937565976.086</v>
+      </c>
+      <c r="H3" s="15">
+        <f t="shared" si="1"/>
+        <v>25677374788949.727</v>
+      </c>
+      <c r="I3" s="15">
+        <f t="shared" si="1"/>
+        <v>23069506690992.805</v>
+      </c>
+      <c r="J3" s="15">
+        <f t="shared" si="1"/>
+        <v>20769204004623.625</v>
+      </c>
+      <c r="K3" s="15">
+        <f t="shared" si="1"/>
+        <v>18700000000000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B5">
+        <v>2021</v>
+      </c>
+      <c r="C5">
+        <f>B5+1</f>
+        <v>2022</v>
+      </c>
+      <c r="D5" s="10">
+        <f t="shared" si="0"/>
+        <v>2023</v>
+      </c>
+      <c r="E5" s="10">
+        <f t="shared" si="0"/>
+        <v>2024</v>
+      </c>
+      <c r="F5" s="10">
+        <f t="shared" si="0"/>
+        <v>2025</v>
+      </c>
+      <c r="G5" s="10">
+        <f t="shared" si="0"/>
+        <v>2026</v>
+      </c>
+      <c r="H5" s="10">
+        <f t="shared" si="0"/>
+        <v>2027</v>
+      </c>
+      <c r="I5" s="10">
+        <f t="shared" si="0"/>
+        <v>2028</v>
+      </c>
+      <c r="J5" s="10">
+        <f t="shared" si="0"/>
+        <v>2029</v>
+      </c>
+      <c r="K5" s="42">
+        <f>J5+1</f>
+        <v>2030</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>332</v>
+      </c>
+      <c r="B6" s="15">
+        <f>B3</f>
+        <v>63680905329200.797</v>
+      </c>
+      <c r="C6" s="10">
+        <f>$B$14*C8+$B$15</f>
+        <v>50.143835563664268</v>
+      </c>
+      <c r="D6" s="10">
+        <f t="shared" ref="D6:J6" si="2">$B$14*D8+$B$15</f>
+        <v>42.225102002311814</v>
+      </c>
+      <c r="E6" s="10">
+        <f t="shared" si="2"/>
+        <v>36.606671127328532</v>
+      </c>
+      <c r="F6" s="10">
+        <f t="shared" si="2"/>
+        <v>32.248677570162016</v>
+      </c>
+      <c r="G6" s="10">
+        <f t="shared" si="2"/>
+        <v>28.687937565976085</v>
+      </c>
+      <c r="H6" s="10">
+        <f t="shared" si="2"/>
+        <v>25.677374788949727</v>
+      </c>
+      <c r="I6" s="10">
+        <f t="shared" si="2"/>
+        <v>23.069506690992803</v>
+      </c>
+      <c r="J6" s="10">
+        <f t="shared" si="2"/>
+        <v>20.769204004623624</v>
+      </c>
+      <c r="K6" s="10">
+        <f>'Long run trend'!B1*44/12</f>
+        <v>18.7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <f>B7+1</f>
+        <v>2</v>
+      </c>
+      <c r="D7" s="10">
+        <f t="shared" ref="D7:J7" si="3">C7+1</f>
+        <v>3</v>
+      </c>
+      <c r="E7" s="10">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="F7" s="10">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="G7" s="10">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="H7" s="10">
+        <f t="shared" si="3"/>
+        <v>7</v>
+      </c>
+      <c r="I7" s="10">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+      <c r="J7" s="10">
+        <f t="shared" si="3"/>
+        <v>9</v>
+      </c>
+      <c r="K7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>339</v>
+      </c>
+      <c r="B8">
+        <f>LN(B7)</f>
+        <v>0</v>
+      </c>
+      <c r="C8" s="10">
+        <f t="shared" ref="C8:J8" si="4">LN(C7)</f>
+        <v>0.69314718055994529</v>
+      </c>
+      <c r="D8" s="10">
+        <f t="shared" si="4"/>
+        <v>1.0986122886681098</v>
+      </c>
+      <c r="E8" s="10">
+        <f t="shared" si="4"/>
+        <v>1.3862943611198906</v>
+      </c>
+      <c r="F8" s="10">
+        <f t="shared" si="4"/>
+        <v>1.6094379124341003</v>
+      </c>
+      <c r="G8" s="10">
+        <f t="shared" si="4"/>
+        <v>1.791759469228055</v>
+      </c>
+      <c r="H8" s="10">
+        <f t="shared" si="4"/>
+        <v>1.9459101490553132</v>
+      </c>
+      <c r="I8" s="10">
+        <f t="shared" si="4"/>
+        <v>2.0794415416798357</v>
+      </c>
+      <c r="J8" s="10">
+        <f t="shared" si="4"/>
+        <v>2.1972245773362196</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B10" s="10">
+        <f>B7</f>
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>336</v>
+      </c>
+      <c r="B11" s="10">
+        <f>B6/1000000000000</f>
+        <v>63.680905329200797</v>
+      </c>
+      <c r="C11">
+        <f t="shared" ref="C11" si="5">K6</f>
+        <v>18.7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>337</v>
+      </c>
+      <c r="B14">
+        <v>-19.53</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>338</v>
+      </c>
+      <c r="B15">
+        <v>63.680999999999997</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -63982,15 +65485,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr>
     <tabColor rgb="FF1F497D"/>
   </sheetPr>
   <dimension ref="A1:AK1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AK2" sqref="B2:AK2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -64120,148 +65623,148 @@
         <v>260</v>
       </c>
       <c r="B2" s="9">
-        <f>Calcs!P28</f>
+        <f>Empirical!P28</f>
         <v>44600000000000</v>
       </c>
       <c r="C2" s="9">
-        <f>Calcs!Q28</f>
-        <v>2614285714285.7144</v>
+        <f>Empirical!Q62</f>
+        <v>10500000000000</v>
       </c>
       <c r="D2" s="9">
-        <f>Calcs!R28</f>
-        <v>23414285714285.711</v>
+        <f>Empirical!R62</f>
+        <v>31300000000000</v>
       </c>
       <c r="E2" s="9">
-        <f>Calcs!S28</f>
-        <v>31214285714285.715</v>
+        <f>Empirical!S62</f>
+        <v>39100000000000</v>
       </c>
       <c r="F2" s="9">
-        <f>Calcs!T28</f>
-        <v>-3085714285714.2856</v>
+        <f>Empirical!T62</f>
+        <v>4800000000000</v>
       </c>
       <c r="G2" s="9">
-        <f>Calcs!U28</f>
-        <v>98814285714285.719</v>
+        <f>Empirical!U62</f>
+        <v>106700000000000</v>
       </c>
       <c r="H2" s="9">
-        <f>Calcs!V28</f>
-        <v>5600000000000</v>
+        <f>Empirical!V62</f>
+        <v>63680905329200.797</v>
       </c>
       <c r="I2" s="9">
-        <f>Calcs!W28</f>
-        <v>5600000000000</v>
+        <f>'Transition to long run trend'!C3</f>
+        <v>50143835563664.266</v>
       </c>
       <c r="J2" s="9">
-        <f>Calcs!X28</f>
-        <v>5600000000000</v>
+        <f>'Transition to long run trend'!D3</f>
+        <v>42225102002311.813</v>
       </c>
       <c r="K2" s="9">
-        <f>Calcs!Y28</f>
-        <v>5600000000000</v>
+        <f>'Transition to long run trend'!E3</f>
+        <v>36606671127328.531</v>
       </c>
       <c r="L2" s="9">
-        <f>Calcs!Z28</f>
-        <v>5600000000000</v>
+        <f>'Transition to long run trend'!F3</f>
+        <v>32248677570162.016</v>
       </c>
       <c r="M2" s="9">
-        <f>Calcs!AA28</f>
-        <v>5600000000000</v>
+        <f>'Transition to long run trend'!G3</f>
+        <v>28687937565976.086</v>
       </c>
       <c r="N2" s="9">
-        <f>Calcs!AB28</f>
-        <v>5600000000000</v>
+        <f>'Transition to long run trend'!H3</f>
+        <v>25677374788949.727</v>
       </c>
       <c r="O2" s="9">
-        <f>Calcs!AC28</f>
-        <v>5600000000000</v>
+        <f>'Transition to long run trend'!I3</f>
+        <v>23069506690992.805</v>
       </c>
       <c r="P2" s="9">
-        <f>Calcs!AD28</f>
-        <v>5600000000000</v>
+        <f>'Transition to long run trend'!J3</f>
+        <v>20769204004623.625</v>
       </c>
       <c r="Q2" s="9">
-        <f>Calcs!AE28</f>
-        <v>5600000000000</v>
+        <f>'Transition to long run trend'!K3</f>
+        <v>18700000000000</v>
       </c>
       <c r="R2" s="9">
-        <f>Calcs!AF28</f>
-        <v>5600000000000</v>
+        <f>'Long run trend'!$B$3</f>
+        <v>18700000000000</v>
       </c>
       <c r="S2" s="9">
-        <f>Calcs!AG28</f>
-        <v>5600000000000</v>
+        <f>'Long run trend'!$B$3</f>
+        <v>18700000000000</v>
       </c>
       <c r="T2" s="9">
-        <f>Calcs!AH28</f>
-        <v>5600000000000</v>
+        <f>'Long run trend'!$B$3</f>
+        <v>18700000000000</v>
       </c>
       <c r="U2" s="9">
-        <f>Calcs!AI28</f>
-        <v>5600000000000</v>
+        <f>'Long run trend'!$B$3</f>
+        <v>18700000000000</v>
       </c>
       <c r="V2" s="9">
-        <f>Calcs!AJ28</f>
-        <v>5600000000000</v>
+        <f>'Long run trend'!$B$3</f>
+        <v>18700000000000</v>
       </c>
       <c r="W2" s="9">
-        <f>Calcs!AK28</f>
-        <v>5600000000000</v>
+        <f>'Long run trend'!$B$3</f>
+        <v>18700000000000</v>
       </c>
       <c r="X2" s="9">
-        <f>Calcs!AL28</f>
-        <v>5600000000000</v>
+        <f>'Long run trend'!$B$3</f>
+        <v>18700000000000</v>
       </c>
       <c r="Y2" s="9">
-        <f>Calcs!AM28</f>
-        <v>5600000000000</v>
+        <f>'Long run trend'!$B$3</f>
+        <v>18700000000000</v>
       </c>
       <c r="Z2" s="9">
-        <f>Calcs!AN28</f>
-        <v>5600000000000</v>
+        <f>'Long run trend'!$B$3</f>
+        <v>18700000000000</v>
       </c>
       <c r="AA2" s="9">
-        <f>Calcs!AO28</f>
-        <v>5600000000000</v>
+        <f>'Long run trend'!$B$3</f>
+        <v>18700000000000</v>
       </c>
       <c r="AB2" s="9">
-        <f>Calcs!AP28</f>
-        <v>5600000000000</v>
+        <f>'Long run trend'!$B$3</f>
+        <v>18700000000000</v>
       </c>
       <c r="AC2" s="9">
-        <f>Calcs!AQ28</f>
-        <v>5600000000000</v>
+        <f>'Long run trend'!$B$3</f>
+        <v>18700000000000</v>
       </c>
       <c r="AD2" s="9">
-        <f>Calcs!AR28</f>
-        <v>5600000000000</v>
+        <f>'Long run trend'!$B$3</f>
+        <v>18700000000000</v>
       </c>
       <c r="AE2" s="9">
-        <f>Calcs!AS28</f>
-        <v>5600000000000</v>
+        <f>'Long run trend'!$B$3</f>
+        <v>18700000000000</v>
       </c>
       <c r="AF2" s="9">
-        <f>Calcs!AT28</f>
-        <v>5600000000000</v>
+        <f>'Long run trend'!$B$3</f>
+        <v>18700000000000</v>
       </c>
       <c r="AG2" s="9">
-        <f>Calcs!AU28</f>
-        <v>5600000000000</v>
+        <f>'Long run trend'!$B$3</f>
+        <v>18700000000000</v>
       </c>
       <c r="AH2" s="9">
-        <f>Calcs!AV28</f>
-        <v>5600000000000</v>
+        <f>'Long run trend'!$B$3</f>
+        <v>18700000000000</v>
       </c>
       <c r="AI2" s="9">
-        <f>Calcs!AW28</f>
-        <v>5600000000000</v>
+        <f>'Long run trend'!$B$3</f>
+        <v>18700000000000</v>
       </c>
       <c r="AJ2" s="9">
-        <f>Calcs!AX28</f>
-        <v>5600000000000</v>
+        <f>'Long run trend'!$B$3</f>
+        <v>18700000000000</v>
       </c>
       <c r="AK2" s="9">
-        <f>Calcs!AY28</f>
-        <v>5600000000000</v>
+        <f>'Long run trend'!$B$3</f>
+        <v>18700000000000</v>
       </c>
     </row>
     <row r="3" spans="1:37" ht="14.5" x14ac:dyDescent="0.35">
@@ -65178,143 +66681,143 @@
       </c>
       <c r="C11" s="9">
         <f>C$2*'data from RPEpUACE'!$B11</f>
-        <v>1736341085.9567566</v>
+        <v>6973828951.7935305</v>
       </c>
       <c r="D11" s="9">
         <f>D$2*'data from RPEpUACE'!$B11</f>
-        <v>15551164152.366795</v>
+        <v>20788652018.203571</v>
       </c>
       <c r="E11" s="9">
         <f>E$2*'data from RPEpUACE'!$B11</f>
-        <v>20731722802.270565</v>
+        <v>25969210668.107338</v>
       </c>
       <c r="F11" s="9">
         <f>F$2*'data from RPEpUACE'!$B11</f>
-        <v>-2049451773.5883029</v>
+        <v>3188036092.2484708</v>
       </c>
       <c r="G11" s="9">
         <f>G$2*'data from RPEpUACE'!$B11</f>
-        <v>65629897768.103203</v>
+        <v>70867385633.939972</v>
       </c>
       <c r="H11" s="9">
         <f>H$2*'data from RPEpUACE'!$B11</f>
-        <v>3719375440.9565496</v>
+        <v>42295213453.447945</v>
       </c>
       <c r="I11" s="9">
         <f>I$2*'data from RPEpUACE'!$B11</f>
-        <v>3719375440.9565496</v>
+        <v>33304241162.652943</v>
       </c>
       <c r="J11" s="9">
         <f>J$2*'data from RPEpUACE'!$B11</f>
-        <v>3719375440.9565496</v>
+        <v>28044822746.300674</v>
       </c>
       <c r="K11" s="9">
         <f>K$2*'data from RPEpUACE'!$B11</f>
-        <v>3719375440.9565496</v>
+        <v>24313205993.956955</v>
       </c>
       <c r="L11" s="9">
         <f>L$2*'data from RPEpUACE'!$B11</f>
-        <v>3719375440.9565496</v>
+        <v>21418739171.033382</v>
       </c>
       <c r="M11" s="9">
         <f>M$2*'data from RPEpUACE'!$B11</f>
-        <v>3719375440.9565496</v>
+        <v>19053787577.604691</v>
       </c>
       <c r="N11" s="9">
         <f>N$2*'data from RPEpUACE'!$B11</f>
-        <v>3719375440.9565496</v>
+        <v>17054249496.117228</v>
       </c>
       <c r="O11" s="9">
         <f>O$2*'data from RPEpUACE'!$B11</f>
-        <v>3719375440.9565496</v>
+        <v>15322170825.260969</v>
       </c>
       <c r="P11" s="9">
         <f>P$2*'data from RPEpUACE'!$B11</f>
-        <v>3719375440.9565496</v>
+        <v>13794369161.252417</v>
       </c>
       <c r="Q11" s="9">
         <f>Q$2*'data from RPEpUACE'!$B11</f>
-        <v>3719375440.9565496</v>
+        <v>12420057276.051334</v>
       </c>
       <c r="R11" s="9">
         <f>R$2*'data from RPEpUACE'!$B11</f>
-        <v>3719375440.9565496</v>
+        <v>12420057276.051334</v>
       </c>
       <c r="S11" s="9">
         <f>S$2*'data from RPEpUACE'!$B11</f>
-        <v>3719375440.9565496</v>
+        <v>12420057276.051334</v>
       </c>
       <c r="T11" s="9">
         <f>T$2*'data from RPEpUACE'!$B11</f>
-        <v>3719375440.9565496</v>
+        <v>12420057276.051334</v>
       </c>
       <c r="U11" s="9">
         <f>U$2*'data from RPEpUACE'!$B11</f>
-        <v>3719375440.9565496</v>
+        <v>12420057276.051334</v>
       </c>
       <c r="V11" s="9">
         <f>V$2*'data from RPEpUACE'!$B11</f>
-        <v>3719375440.9565496</v>
+        <v>12420057276.051334</v>
       </c>
       <c r="W11" s="9">
         <f>W$2*'data from RPEpUACE'!$B11</f>
-        <v>3719375440.9565496</v>
+        <v>12420057276.051334</v>
       </c>
       <c r="X11" s="9">
         <f>X$2*'data from RPEpUACE'!$B11</f>
-        <v>3719375440.9565496</v>
+        <v>12420057276.051334</v>
       </c>
       <c r="Y11" s="9">
         <f>Y$2*'data from RPEpUACE'!$B11</f>
-        <v>3719375440.9565496</v>
+        <v>12420057276.051334</v>
       </c>
       <c r="Z11" s="9">
         <f>Z$2*'data from RPEpUACE'!$B11</f>
-        <v>3719375440.9565496</v>
+        <v>12420057276.051334</v>
       </c>
       <c r="AA11" s="9">
         <f>AA$2*'data from RPEpUACE'!$B11</f>
-        <v>3719375440.9565496</v>
+        <v>12420057276.051334</v>
       </c>
       <c r="AB11" s="9">
         <f>AB$2*'data from RPEpUACE'!$B11</f>
-        <v>3719375440.9565496</v>
+        <v>12420057276.051334</v>
       </c>
       <c r="AC11" s="9">
         <f>AC$2*'data from RPEpUACE'!$B11</f>
-        <v>3719375440.9565496</v>
+        <v>12420057276.051334</v>
       </c>
       <c r="AD11" s="9">
         <f>AD$2*'data from RPEpUACE'!$B11</f>
-        <v>3719375440.9565496</v>
+        <v>12420057276.051334</v>
       </c>
       <c r="AE11" s="9">
         <f>AE$2*'data from RPEpUACE'!$B11</f>
-        <v>3719375440.9565496</v>
+        <v>12420057276.051334</v>
       </c>
       <c r="AF11" s="9">
         <f>AF$2*'data from RPEpUACE'!$B11</f>
-        <v>3719375440.9565496</v>
+        <v>12420057276.051334</v>
       </c>
       <c r="AG11" s="9">
         <f>AG$2*'data from RPEpUACE'!$B11</f>
-        <v>3719375440.9565496</v>
+        <v>12420057276.051334</v>
       </c>
       <c r="AH11" s="9">
         <f>AH$2*'data from RPEpUACE'!$B11</f>
-        <v>3719375440.9565496</v>
+        <v>12420057276.051334</v>
       </c>
       <c r="AI11" s="9">
         <f>AI$2*'data from RPEpUACE'!$B11</f>
-        <v>3719375440.9565496</v>
+        <v>12420057276.051334</v>
       </c>
       <c r="AJ11" s="9">
         <f>AJ$2*'data from RPEpUACE'!$B11</f>
-        <v>3719375440.9565496</v>
+        <v>12420057276.051334</v>
       </c>
       <c r="AK11" s="9">
         <f>AK$2*'data from RPEpUACE'!$B11</f>
-        <v>3719375440.9565496</v>
+        <v>12420057276.051334</v>
       </c>
     </row>
     <row r="12" spans="1:37" ht="14.5" x14ac:dyDescent="0.35">
@@ -65327,143 +66830,143 @@
       </c>
       <c r="C12" s="9">
         <f>C$2*'data from RPEpUACE'!$B12</f>
-        <v>100726716.70259315</v>
+        <v>404558124.46123475</v>
       </c>
       <c r="D12" s="9">
         <f>D$2*'data from RPEpUACE'!$B12</f>
-        <v>902137096.58770573</v>
+        <v>1205968504.3463473</v>
       </c>
       <c r="E12" s="9">
         <f>E$2*'data from RPEpUACE'!$B12</f>
-        <v>1202665989.0446231</v>
+        <v>1506497396.8032646</v>
       </c>
       <c r="F12" s="9">
         <f>F$2*'data from RPEpUACE'!$B12</f>
-        <v>-118890550.86207715</v>
+        <v>184940856.89656445</v>
       </c>
       <c r="G12" s="9">
         <f>G$2*'data from RPEpUACE'!$B12</f>
-        <v>3807249723.6712394</v>
+        <v>4111081131.4298811</v>
       </c>
       <c r="H12" s="9">
         <f>H$2*'data from RPEpUACE'!$B12</f>
-        <v>215764333.04599187</v>
+        <v>2453583583.2357073</v>
       </c>
       <c r="I12" s="9">
         <f>I$2*'data from RPEpUACE'!$B12</f>
-        <v>215764333.04599187</v>
+        <v>1932009149.4217694</v>
       </c>
       <c r="J12" s="9">
         <f>J$2*'data from RPEpUACE'!$B12</f>
-        <v>215764333.04599187</v>
+        <v>1626905530.5942471</v>
       </c>
       <c r="K12" s="9">
         <f>K$2*'data from RPEpUACE'!$B12</f>
-        <v>215764333.04599187</v>
+        <v>1410431068.0039301</v>
       </c>
       <c r="L12" s="9">
         <f>L$2*'data from RPEpUACE'!$B12</f>
-        <v>215764333.04599187</v>
+        <v>1242520429.9180794</v>
       </c>
       <c r="M12" s="9">
         <f>M$2*'data from RPEpUACE'!$B12</f>
-        <v>215764333.04599187</v>
+        <v>1105327449.1764081</v>
       </c>
       <c r="N12" s="9">
         <f>N$2*'data from RPEpUACE'!$B12</f>
-        <v>215764333.04599187</v>
+        <v>989332436.73387575</v>
       </c>
       <c r="O12" s="9">
         <f>O$2*'data from RPEpUACE'!$B12</f>
-        <v>215764333.04599187</v>
+        <v>888852986.58609092</v>
       </c>
       <c r="P12" s="9">
         <f>P$2*'data from RPEpUACE'!$B12</f>
-        <v>215764333.04599187</v>
+        <v>800223830.34888577</v>
       </c>
       <c r="Q12" s="9">
         <f>Q$2*'data from RPEpUACE'!$B12</f>
-        <v>215764333.04599187</v>
+        <v>720498754.99286568</v>
       </c>
       <c r="R12" s="9">
         <f>R$2*'data from RPEpUACE'!$B12</f>
-        <v>215764333.04599187</v>
+        <v>720498754.99286568</v>
       </c>
       <c r="S12" s="9">
         <f>S$2*'data from RPEpUACE'!$B12</f>
-        <v>215764333.04599187</v>
+        <v>720498754.99286568</v>
       </c>
       <c r="T12" s="9">
         <f>T$2*'data from RPEpUACE'!$B12</f>
-        <v>215764333.04599187</v>
+        <v>720498754.99286568</v>
       </c>
       <c r="U12" s="9">
         <f>U$2*'data from RPEpUACE'!$B12</f>
-        <v>215764333.04599187</v>
+        <v>720498754.99286568</v>
       </c>
       <c r="V12" s="9">
         <f>V$2*'data from RPEpUACE'!$B12</f>
-        <v>215764333.04599187</v>
+        <v>720498754.99286568</v>
       </c>
       <c r="W12" s="9">
         <f>W$2*'data from RPEpUACE'!$B12</f>
-        <v>215764333.04599187</v>
+        <v>720498754.99286568</v>
       </c>
       <c r="X12" s="9">
         <f>X$2*'data from RPEpUACE'!$B12</f>
-        <v>215764333.04599187</v>
+        <v>720498754.99286568</v>
       </c>
       <c r="Y12" s="9">
         <f>Y$2*'data from RPEpUACE'!$B12</f>
-        <v>215764333.04599187</v>
+        <v>720498754.99286568</v>
       </c>
       <c r="Z12" s="9">
         <f>Z$2*'data from RPEpUACE'!$B12</f>
-        <v>215764333.04599187</v>
+        <v>720498754.99286568</v>
       </c>
       <c r="AA12" s="9">
         <f>AA$2*'data from RPEpUACE'!$B12</f>
-        <v>215764333.04599187</v>
+        <v>720498754.99286568</v>
       </c>
       <c r="AB12" s="9">
         <f>AB$2*'data from RPEpUACE'!$B12</f>
-        <v>215764333.04599187</v>
+        <v>720498754.99286568</v>
       </c>
       <c r="AC12" s="9">
         <f>AC$2*'data from RPEpUACE'!$B12</f>
-        <v>215764333.04599187</v>
+        <v>720498754.99286568</v>
       </c>
       <c r="AD12" s="9">
         <f>AD$2*'data from RPEpUACE'!$B12</f>
-        <v>215764333.04599187</v>
+        <v>720498754.99286568</v>
       </c>
       <c r="AE12" s="9">
         <f>AE$2*'data from RPEpUACE'!$B12</f>
-        <v>215764333.04599187</v>
+        <v>720498754.99286568</v>
       </c>
       <c r="AF12" s="9">
         <f>AF$2*'data from RPEpUACE'!$B12</f>
-        <v>215764333.04599187</v>
+        <v>720498754.99286568</v>
       </c>
       <c r="AG12" s="9">
         <f>AG$2*'data from RPEpUACE'!$B12</f>
-        <v>215764333.04599187</v>
+        <v>720498754.99286568</v>
       </c>
       <c r="AH12" s="9">
         <f>AH$2*'data from RPEpUACE'!$B12</f>
-        <v>215764333.04599187</v>
+        <v>720498754.99286568</v>
       </c>
       <c r="AI12" s="9">
         <f>AI$2*'data from RPEpUACE'!$B12</f>
-        <v>215764333.04599187</v>
+        <v>720498754.99286568</v>
       </c>
       <c r="AJ12" s="9">
         <f>AJ$2*'data from RPEpUACE'!$B12</f>
-        <v>215764333.04599187</v>
+        <v>720498754.99286568</v>
       </c>
       <c r="AK12" s="9">
         <f>AK$2*'data from RPEpUACE'!$B12</f>
-        <v>215764333.04599187</v>
+        <v>720498754.99286568</v>
       </c>
     </row>
     <row r="13" spans="1:37" ht="14.5" x14ac:dyDescent="0.35">

</xml_diff>